<commit_message>
some file reorganization, and added new graphing and analyses
added confound graphs to LG_confound_analysis
</commit_message>
<xml_diff>
--- a/LG_ages_5.xlsx
+++ b/LG_ages_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B033250-9E7B-3847-96F8-3A1EC5E288FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C004BB-76D0-4149-99B9-ABD14DEA8931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{64B086B9-4742-394D-83A6-C568D1A84796}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>blg064</t>
+  </si>
+  <si>
+    <t>blg077</t>
+  </si>
+  <si>
+    <t>blg085</t>
   </si>
 </sst>
 </file>
@@ -743,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7DBEF7-64BA-CC45-9F01-8C0388F0C6F2}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1345,31 +1351,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" t="s">
-        <v>38</v>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="3">
+        <v>5</v>
+      </c>
+      <c r="C55" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B56" s="3">
+        <v>5</v>
+      </c>
+      <c r="C56" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>38</v>
@@ -1380,7 +1386,7 @@
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>38</v>
@@ -1390,8 +1396,8 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>42</v>
+      <c r="A59" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>38</v>
@@ -1402,7 +1408,7 @@
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>38</v>
@@ -1412,8 +1418,8 @@
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>44</v>
+      <c r="A61" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>38</v>
@@ -1424,29 +1430,29 @@
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>38</v>
@@ -1457,7 +1463,7 @@
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>38</v>
@@ -1468,7 +1474,7 @@
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>38</v>
@@ -1479,7 +1485,7 @@
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>38</v>
@@ -1490,7 +1496,7 @@
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>38</v>
@@ -1501,7 +1507,7 @@
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>38</v>
@@ -1512,7 +1518,7 @@
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>38</v>
@@ -1523,7 +1529,7 @@
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>38</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>38</v>
@@ -1545,7 +1551,7 @@
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>38</v>
@@ -1556,7 +1562,7 @@
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>38</v>
@@ -1567,7 +1573,7 @@
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>38</v>
@@ -1578,7 +1584,7 @@
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>38</v>
@@ -1589,7 +1595,7 @@
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>38</v>
@@ -1600,7 +1606,7 @@
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>38</v>
@@ -1611,7 +1617,7 @@
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>38</v>
@@ -1622,7 +1628,7 @@
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>38</v>
@@ -1633,7 +1639,7 @@
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>38</v>
@@ -1644,7 +1650,7 @@
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>38</v>
@@ -1655,7 +1661,7 @@
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>38</v>
@@ -1666,7 +1672,7 @@
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>38</v>
@@ -1677,7 +1683,7 @@
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>38</v>
@@ -1688,7 +1694,7 @@
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>38</v>
@@ -1699,7 +1705,7 @@
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>38</v>
@@ -1710,7 +1716,7 @@
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>38</v>
@@ -1721,7 +1727,7 @@
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>38</v>
@@ -1732,7 +1738,7 @@
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>38</v>
@@ -1743,7 +1749,7 @@
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>38</v>
@@ -1754,7 +1760,7 @@
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>38</v>
@@ -1765,7 +1771,7 @@
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>38</v>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>38</v>
@@ -1787,18 +1793,40 @@
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C95" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B95" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B97" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C95">
-    <sortCondition ref="A2:A95"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C97">
+    <sortCondition ref="A2:A97"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding data files and code to analyze bko2 full paradigm
</commit_message>
<xml_diff>
--- a/LG_ages_5.xlsx
+++ b/LG_ages_5.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C004BB-76D0-4149-99B9-ABD14DEA8931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6F0BD-0F50-CA4E-9050-70F5569693B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{64B086B9-4742-394D-83A6-C568D1A84796}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -751,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7DBEF7-64BA-CC45-9F01-8C0388F0C6F2}">
   <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,31 +779,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="B3" s="3">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="B4" s="3">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -812,20 +812,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="B6" s="3">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
@@ -835,19 +835,19 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="A8" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="B8" s="3">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3">
         <v>5</v>
@@ -856,130 +856,130 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="3">
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="3">
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="3">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2">
+        <v>8</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="3">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="3">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="3">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="3">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="3">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="2">
-        <v>11</v>
-      </c>
-      <c r="C18" t="s">
-        <v>14</v>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="3">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="B19" s="2">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>16</v>
+      <c r="A20" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B20" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>17</v>
+      <c r="A21" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B21" s="3">
         <v>8</v>
@@ -989,77 +989,77 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>18</v>
+      <c r="A22" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="3">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>19</v>
+      <c r="A23" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B23" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B24" s="3">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="B25" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>22</v>
+      <c r="A26" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B26" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B27" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B28" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1067,10 +1067,10 @@
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B29" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1078,21 +1078,21 @@
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1100,142 +1100,142 @@
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="3">
-        <v>6</v>
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="2">
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>86</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B34" s="3">
-        <v>5</v>
-      </c>
-      <c r="C34">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B35" s="3">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="2">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="B36" s="3">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="2">
-        <v>10</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="3">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="2">
-        <v>7</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B38" s="3">
+        <v>9</v>
+      </c>
+      <c r="C38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="2">
-        <v>6</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="B39" s="3">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="2">
-        <v>6</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="B40" s="3">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="3">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="2">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B43" s="2">
         <v>9</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="C43" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B44" s="3">
         <v>11</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="3">
-        <v>11</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="3">
-        <v>9</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B45" s="3">
         <v>11</v>
@@ -1254,10 +1254,10 @@
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B46" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
@@ -1265,7 +1265,7 @@
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B47" s="3">
         <v>11</v>
@@ -1275,30 +1275,30 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="3">
+        <v>11</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" s="3">
+        <v>11</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B48" s="3">
-        <v>9</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" s="3">
-        <v>9</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>96</v>
       </c>
       <c r="B50" s="3">
         <v>9</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52" s="3">
         <v>9</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B53" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>14</v>
@@ -1342,7 +1342,7 @@
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" s="3">
         <v>9</v>
@@ -1351,26 +1351,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>101</v>
+    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>99</v>
       </c>
       <c r="B55" s="3">
-        <v>5</v>
-      </c>
-      <c r="C55" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="5" t="s">
-        <v>102</v>
+        <v>10</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>100</v>
       </c>
       <c r="B56" s="3">
-        <v>5</v>
-      </c>
-      <c r="C56" s="3">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1826,7 +1826,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C97">
-    <sortCondition ref="A2:A97"/>
+    <sortCondition ref="C2:C97"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new markdown file called bko1 thesis analysis which will be the one stop shop for all bko1 analyses including LG BK correlation
</commit_message>
<xml_diff>
--- a/LG_ages_5.xlsx
+++ b/LG_ages_5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A6F0BD-0F50-CA4E-9050-70F5569693B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FD9A8C-ACB5-E045-BC8A-97981F27B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{64B086B9-4742-394D-83A6-C568D1A84796}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -345,6 +345,21 @@
   </si>
   <si>
     <t>blg085</t>
+  </si>
+  <si>
+    <t>blg087</t>
+  </si>
+  <si>
+    <t>blg088</t>
+  </si>
+  <si>
+    <t>blg092</t>
+  </si>
+  <si>
+    <t>blg095</t>
+  </si>
+  <si>
+    <t>blg097</t>
   </si>
 </sst>
 </file>
@@ -749,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7DBEF7-64BA-CC45-9F01-8C0388F0C6F2}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,6 +1837,61 @@
       </c>
       <c r="C97" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B98" s="3">
+        <v>5</v>
+      </c>
+      <c r="C98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B99" s="3">
+        <v>5</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B100" s="3">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="3">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="3">
+        <v>5</v>
+      </c>
+      <c r="C102">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding graphing for the number of local elements
</commit_message>
<xml_diff>
--- a/LG_ages_5.xlsx
+++ b/LG_ages_5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisabeth/Desktop/UMASS/BKonline data/BK-Online-Replication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FD9A8C-ACB5-E045-BC8A-97981F27B99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63853040-53A2-9146-BC29-017534C9A44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{64B086B9-4742-394D-83A6-C568D1A84796}"/>
+    <workbookView xWindow="29380" yWindow="840" windowWidth="28800" windowHeight="16420" xr2:uid="{64B086B9-4742-394D-83A6-C568D1A84796}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7DBEF7-64BA-CC45-9F01-8C0388F0C6F2}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,31 +794,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>94</v>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="3">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3">
         <v>5</v>
@@ -827,20 +827,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>87</v>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B7" s="3">
         <v>5</v>
@@ -850,151 +850,151 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>89</v>
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="3">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="3">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="3">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B16" s="3">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
         <v>7</v>
       </c>
-      <c r="B13" s="3">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="3">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="3">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="2">
-        <v>8</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="2">
-        <v>7</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
+      <c r="C17" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>34</v>
+      <c r="A18" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B18" s="2">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
         <v>6</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="3">
-        <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>5</v>
+      <c r="A21" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B21" s="3">
         <v>8</v>
@@ -1004,77 +1004,77 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
+      <c r="A22" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B22" s="3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
+      <c r="A23" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B23" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B24" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>11</v>
+      <c r="A25" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B25" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>12</v>
+      <c r="A26" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B26" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B27" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B28" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
@@ -1082,10 +1082,10 @@
     </row>
     <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C29" t="s">
         <v>4</v>
@@ -1093,21 +1093,21 @@
     </row>
     <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B31" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
@@ -1115,142 +1115,142 @@
     </row>
     <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="2">
-        <v>11</v>
+      <c r="A33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3">
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="B34" s="3">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B35" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B36" s="3">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2">
+        <v>8</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="2">
         <v>10</v>
       </c>
-      <c r="C36" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="3">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="3">
-        <v>9</v>
-      </c>
-      <c r="C38" t="s">
-        <v>14</v>
+        <v>33</v>
+      </c>
+      <c r="B38" s="2">
+        <v>7</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="3">
-        <v>11</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="B39" s="2">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B40" s="3">
-        <v>11</v>
-      </c>
-      <c r="C40" t="s">
-        <v>14</v>
+        <v>35</v>
+      </c>
+      <c r="B40" s="2">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="3">
+        <v>36</v>
+      </c>
+      <c r="B41" s="2">
         <v>9</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="2">
-        <v>10</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="A42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="3">
+        <v>11</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="A43" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="3">
+        <v>11</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="3">
         <v>9</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" s="3">
-        <v>11</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>14</v>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="45" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B45" s="3">
         <v>11</v>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="46" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B46" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>14</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="47" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B47" s="3">
         <v>11</v>
@@ -1290,30 +1290,30 @@
       </c>
     </row>
     <row r="48" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
-        <v>83</v>
+      <c r="A48" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B48" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
-        <v>84</v>
+      <c r="A49" t="s">
+        <v>95</v>
       </c>
       <c r="B49" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>85</v>
+      <c r="A50" t="s">
+        <v>96</v>
       </c>
       <c r="B50" s="3">
         <v>9</v>
@@ -1324,10 +1324,10 @@
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B51" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>14</v>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B52" s="3">
         <v>9</v>
@@ -1346,10 +1346,10 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B53" s="3">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>14</v>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="54" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B54" s="3">
         <v>9</v>
@@ -1366,86 +1366,86 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>99</v>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="B55" s="3">
-        <v>10</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>100</v>
+        <v>5</v>
+      </c>
+      <c r="C55" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>102</v>
       </c>
       <c r="B56" s="3">
-        <v>9</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="C56" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
+      <c r="A57" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="3">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C58" t="s">
-        <v>38</v>
+      <c r="A58" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B58" s="3">
+        <v>5</v>
+      </c>
+      <c r="C58">
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C59" t="s">
-        <v>38</v>
+      <c r="A59" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="3">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C60" t="s">
-        <v>38</v>
+      <c r="A60" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="3">
+        <v>5</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C61" t="s">
-        <v>38</v>
+        <v>107</v>
+      </c>
+      <c r="B61" s="3">
+        <v>5</v>
+      </c>
+      <c r="C61">
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>38</v>
@@ -1456,7 +1456,7 @@
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>38</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>38</v>
@@ -1477,8 +1477,8 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>46</v>
+      <c r="A65" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>38</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>38</v>
@@ -1499,8 +1499,8 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>48</v>
+      <c r="A67" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>38</v>
@@ -1510,8 +1510,8 @@
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
-        <v>49</v>
+      <c r="A68" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>38</v>
@@ -1521,8 +1521,8 @@
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>50</v>
+      <c r="A69" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>38</v>
@@ -1533,7 +1533,7 @@
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>38</v>
@@ -1544,7 +1544,7 @@
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>38</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>38</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>38</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>38</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>38</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B76" s="3" t="s">
         <v>38</v>
@@ -1610,7 +1610,7 @@
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B77" s="3" t="s">
         <v>38</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>38</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>38</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>38</v>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>38</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>38</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>38</v>
@@ -1687,7 +1687,7 @@
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>38</v>
@@ -1698,7 +1698,7 @@
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>38</v>
@@ -1709,7 +1709,7 @@
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>38</v>
@@ -1720,7 +1720,7 @@
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>38</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>38</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>38</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B90" s="3" t="s">
         <v>38</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>38</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>38</v>
@@ -1786,7 +1786,7 @@
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>38</v>
@@ -1797,7 +1797,7 @@
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>38</v>
@@ -1808,7 +1808,7 @@
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>38</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>38</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B97" s="3" t="s">
         <v>38</v>
@@ -1841,62 +1841,62 @@
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B98" s="3">
-        <v>5</v>
-      </c>
-      <c r="C98">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B99" s="3">
-        <v>5</v>
-      </c>
-      <c r="C99">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B100" s="3">
-        <v>5</v>
-      </c>
-      <c r="C100">
-        <v>5</v>
+        <v>76</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C100" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B101" s="3">
-        <v>5</v>
-      </c>
-      <c r="C101">
-        <v>5</v>
+        <v>77</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B102" s="3">
-        <v>5</v>
-      </c>
-      <c r="C102">
-        <v>5</v>
+        <v>78</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C102" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C97">
-    <sortCondition ref="C2:C97"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C103">
+    <sortCondition ref="A2:A103"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>